<commit_message>
Added a string splitting function
</commit_message>
<xml_diff>
--- a/ExcelStuff/TESTCOPY.xlsx
+++ b/ExcelStuff/TESTCOPY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danma\Documents\GitHub\JDJ-1\ExcelStuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeo\Documents\GitHub\JDJ-1\ExcelStuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07D6AF67-315C-4D6F-A941-ED4FE95AAB8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E378C6F4-2345-4B84-A984-4C58650BA169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TESTCOPY" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1253,14 +1253,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1298,7 +1310,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1330,7 +1342,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1362,7 +1374,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1394,7 +1406,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1426,7 +1438,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1458,7 +1470,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1490,7 +1502,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1522,7 +1534,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1554,7 +1566,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1586,7 +1598,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1618,7 +1630,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1650,7 +1662,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1682,7 +1694,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1714,7 +1726,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1746,7 +1758,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1778,7 +1790,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1810,7 +1822,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1842,7 +1854,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1874,7 +1886,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -1906,7 +1918,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -1938,7 +1950,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -1970,7 +1982,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -2002,7 +2014,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -2034,7 +2046,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -2066,7 +2078,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -2098,7 +2110,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -2130,7 +2142,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -2162,7 +2174,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -2194,7 +2206,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2226,7 +2238,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -2258,7 +2270,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -2290,7 +2302,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -2322,7 +2334,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -2354,7 +2366,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -2386,7 +2398,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -2418,7 +2430,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>89</v>
       </c>
@@ -2450,7 +2462,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -2482,7 +2494,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -2514,7 +2526,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>95</v>
       </c>
@@ -2546,7 +2558,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -2578,7 +2590,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -2610,7 +2622,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>101</v>
       </c>
@@ -2642,7 +2654,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -2674,7 +2686,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -2706,7 +2718,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -2738,7 +2750,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -2770,7 +2782,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -2802,7 +2814,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -2834,7 +2846,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>115</v>
       </c>
@@ -2866,7 +2878,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>117</v>
       </c>
@@ -2898,7 +2910,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>119</v>
       </c>
@@ -2930,7 +2942,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>121</v>
       </c>
@@ -2962,7 +2974,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>123</v>
       </c>
@@ -2994,7 +3006,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>125</v>
       </c>
@@ -3026,7 +3038,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>127</v>
       </c>
@@ -3058,7 +3070,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>129</v>
       </c>

</xml_diff>